<commit_message>
Fix minor errors on dataset
</commit_message>
<xml_diff>
--- a/data/data_processed.xlsx
+++ b/data/data_processed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mexis\OneDrive\Υπολογιστής\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mexis\OneDrive\Υπολογιστής\dynamic-modeling\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F74E741C-F4C7-45B3-A9F1-9DF309E0B9AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57A272CF-3C48-4460-901F-F19EF8661FBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{C50486F1-D1DE-4E23-A44E-59CA489FDBF3}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{C50486F1-D1DE-4E23-A44E-59CA489FDBF3}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw data" sheetId="3" r:id="rId1"/>
@@ -1443,22 +1443,22 @@
     <xf numFmtId="2" fontId="17" fillId="37" borderId="0" xfId="34" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="17" fillId="37" borderId="0" xfId="34" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="108" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="10" xfId="108" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="10" xfId="108" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="10" xfId="108" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="37" borderId="10" xfId="108" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="10" xfId="108" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="36" borderId="10" xfId="108" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="10" xfId="108" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="10" xfId="108" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="36" borderId="10" xfId="108" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="108" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
@@ -1908,8 +1908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96C23BC7-A187-4678-9EC0-A3C5E1658A31}">
   <dimension ref="A1:L207"/>
   <sheetViews>
-    <sheetView topLeftCell="A164" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B154" sqref="B154"/>
+    <sheetView tabSelected="1" topLeftCell="A148" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H160" sqref="H160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1955,7 +1955,7 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="101" t="s">
+      <c r="A2" s="99" t="s">
         <v>105</v>
       </c>
       <c r="B2" s="11">
@@ -1985,9 +1985,9 @@
       <c r="L2" s="75"/>
     </row>
     <row r="3" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="101"/>
+      <c r="A3" s="99"/>
       <c r="B3" s="11">
-        <v>0.48333333333333162</v>
+        <v>0.48</v>
       </c>
       <c r="C3" s="12">
         <v>7.87</v>
@@ -2013,9 +2013,9 @@
       <c r="L3" s="75"/>
     </row>
     <row r="4" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="101"/>
+      <c r="A4" s="99"/>
       <c r="B4" s="11">
-        <v>0.93333333333333268</v>
+        <v>0.93</v>
       </c>
       <c r="C4" s="12">
         <v>7.94</v>
@@ -2041,9 +2041,9 @@
       <c r="L4" s="75"/>
     </row>
     <row r="5" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="101"/>
+      <c r="A5" s="99"/>
       <c r="B5" s="11">
-        <v>1.5499999999999985</v>
+        <v>1.55</v>
       </c>
       <c r="C5" s="12">
         <v>7.22</v>
@@ -2069,9 +2069,9 @@
       <c r="L5" s="75"/>
     </row>
     <row r="6" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="101"/>
+      <c r="A6" s="99"/>
       <c r="B6" s="11">
-        <v>2.2666666666666653</v>
+        <v>2.27</v>
       </c>
       <c r="C6" s="12">
         <v>6.51</v>
@@ -2097,9 +2097,9 @@
       <c r="L6" s="75"/>
     </row>
     <row r="7" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="101"/>
+      <c r="A7" s="99"/>
       <c r="B7" s="11">
-        <v>3.0333333333333319</v>
+        <v>3.03</v>
       </c>
       <c r="C7" s="12">
         <v>4.6999999999999993</v>
@@ -2125,9 +2125,9 @@
       <c r="L7" s="75"/>
     </row>
     <row r="8" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="101"/>
+      <c r="A8" s="99"/>
       <c r="B8" s="11">
-        <v>3.5833333333333321</v>
+        <v>3.58</v>
       </c>
       <c r="C8" s="12">
         <v>2.82</v>
@@ -2153,9 +2153,9 @@
       <c r="L8" s="75"/>
     </row>
     <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="101"/>
+      <c r="A9" s="99"/>
       <c r="B9" s="11">
-        <v>4.0833333333333304</v>
+        <v>4.08</v>
       </c>
       <c r="C9" s="12">
         <v>1.2E-2</v>
@@ -2181,11 +2181,11 @@
       <c r="L9" s="75"/>
     </row>
     <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="101" t="s">
+      <c r="A10" s="99" t="s">
         <v>104</v>
       </c>
       <c r="B10" s="12">
-        <v>4.7333333333333307</v>
+        <v>4.7300000000000004</v>
       </c>
       <c r="C10" s="12">
         <v>1.2999999999999999E-2</v>
@@ -2211,9 +2211,9 @@
       <c r="L10" s="75"/>
     </row>
     <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="101"/>
+      <c r="A11" s="99"/>
       <c r="B11" s="12">
-        <v>5.2833333333333314</v>
+        <v>5.28</v>
       </c>
       <c r="C11" s="12">
         <v>1.4E-2</v>
@@ -2239,9 +2239,9 @@
       <c r="L11" s="75"/>
     </row>
     <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="101"/>
+      <c r="A12" s="99"/>
       <c r="B12" s="12">
-        <v>6.3166666666666664</v>
+        <v>6.32</v>
       </c>
       <c r="C12" s="12">
         <v>1.2E-2</v>
@@ -2267,9 +2267,9 @@
       <c r="L12" s="75"/>
     </row>
     <row r="13" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="101"/>
+      <c r="A13" s="99"/>
       <c r="B13" s="12">
-        <v>7.0166666666666639</v>
+        <v>7.02</v>
       </c>
       <c r="C13" s="12">
         <v>8.9999999999999993E-3</v>
@@ -2295,9 +2295,9 @@
       <c r="L13" s="75"/>
     </row>
     <row r="14" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="101"/>
+      <c r="A14" s="99"/>
       <c r="B14" s="12">
-        <v>7.5500000000000007</v>
+        <v>7.55</v>
       </c>
       <c r="C14" s="12">
         <v>1.6E-2</v>
@@ -2323,9 +2323,9 @@
       <c r="L14" s="75"/>
     </row>
     <row r="15" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="101"/>
+      <c r="A15" s="99"/>
       <c r="B15" s="12">
-        <v>8.0166666666666657</v>
+        <v>8.02</v>
       </c>
       <c r="C15" s="12">
         <v>1.2E-2</v>
@@ -2351,9 +2351,9 @@
       <c r="L15" s="75"/>
     </row>
     <row r="16" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="101"/>
+      <c r="A16" s="99"/>
       <c r="B16" s="12">
-        <v>8.4833333333333343</v>
+        <v>8.48</v>
       </c>
       <c r="C16" s="12">
         <v>1.4E-2</v>
@@ -2379,9 +2379,9 @@
       <c r="L16" s="75"/>
     </row>
     <row r="17" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="101"/>
+      <c r="A17" s="99"/>
       <c r="B17" s="12">
-        <v>8.8499999999999961</v>
+        <v>8.85</v>
       </c>
       <c r="C17" s="12">
         <v>8.0000000000000002E-3</v>
@@ -2407,9 +2407,9 @@
       <c r="L17" s="75"/>
     </row>
     <row r="18" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="101"/>
+      <c r="A18" s="99"/>
       <c r="B18" s="12">
-        <v>9.216666666666665</v>
+        <v>9.2200000000000006</v>
       </c>
       <c r="C18" s="12">
         <v>4.0000000000000001E-3</v>
@@ -2435,7 +2435,7 @@
       <c r="L18" s="75"/>
     </row>
     <row r="19" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="101"/>
+      <c r="A19" s="99"/>
       <c r="B19" s="12">
         <v>9.5</v>
       </c>
@@ -2463,7 +2463,7 @@
       <c r="L19" s="74"/>
     </row>
     <row r="20" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="101"/>
+      <c r="A20" s="99"/>
       <c r="B20" s="15">
         <v>10</v>
       </c>
@@ -2491,7 +2491,7 @@
       <c r="L20" s="74"/>
     </row>
     <row r="21" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="102" t="s">
+      <c r="A21" s="101" t="s">
         <v>105</v>
       </c>
       <c r="B21" s="22">
@@ -2521,9 +2521,9 @@
       <c r="L21" s="74"/>
     </row>
     <row r="22" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="102"/>
+      <c r="A22" s="101"/>
       <c r="B22" s="22">
-        <v>0.8333333333333357</v>
+        <v>0.83333330000000005</v>
       </c>
       <c r="C22" s="23">
         <v>7.95</v>
@@ -2549,9 +2549,9 @@
       <c r="L22" s="74"/>
     </row>
     <row r="23" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="102"/>
+      <c r="A23" s="101"/>
       <c r="B23" s="22">
-        <v>1.6166666666666654</v>
+        <v>1.6166666999999999</v>
       </c>
       <c r="C23" s="23">
         <v>6.7600000000000007</v>
@@ -2578,9 +2578,9 @@
       <c r="L23" s="74"/>
     </row>
     <row r="24" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="102"/>
+      <c r="A24" s="101"/>
       <c r="B24" s="22">
-        <v>3.3833333333333382</v>
+        <v>3.3833332999999999</v>
       </c>
       <c r="C24" s="23">
         <v>0.36499999999999999</v>
@@ -2607,11 +2607,11 @@
       <c r="L24" s="74"/>
     </row>
     <row r="25" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="102" t="s">
+      <c r="A25" s="101" t="s">
         <v>104</v>
       </c>
       <c r="B25" s="22">
-        <v>4.1166666666666689</v>
+        <v>4.1166666999999997</v>
       </c>
       <c r="C25" s="23">
         <v>1.0999999999999999E-2</v>
@@ -2638,9 +2638,9 @@
       <c r="L25" s="74"/>
     </row>
     <row r="26" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="102"/>
+      <c r="A26" s="101"/>
       <c r="B26" s="22">
-        <v>5.7333333333333343</v>
+        <v>5.7333333</v>
       </c>
       <c r="C26" s="23">
         <v>0</v>
@@ -2667,9 +2667,9 @@
       <c r="L26" s="74"/>
     </row>
     <row r="27" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="102"/>
+      <c r="A27" s="101"/>
       <c r="B27" s="22">
-        <v>6.5333333333333332</v>
+        <v>6.5333332999999998</v>
       </c>
       <c r="C27" s="23">
         <v>0</v>
@@ -2696,9 +2696,9 @@
       <c r="L27" s="74"/>
     </row>
     <row r="28" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="102"/>
+      <c r="A28" s="101"/>
       <c r="B28" s="22">
-        <v>7.4000000000000039</v>
+        <v>7.4</v>
       </c>
       <c r="C28" s="23">
         <v>0.01</v>
@@ -2724,9 +2724,9 @@
       <c r="L28" s="74"/>
     </row>
     <row r="29" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="102"/>
+      <c r="A29" s="101"/>
       <c r="B29" s="22">
-        <v>8.0000000000000018</v>
+        <v>8</v>
       </c>
       <c r="C29" s="23">
         <v>0</v>
@@ -2752,11 +2752,11 @@
       <c r="L29" s="8"/>
     </row>
     <row r="30" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="102" t="s">
+      <c r="A30" s="101" t="s">
         <v>103</v>
       </c>
       <c r="B30" s="22">
-        <v>9.2833333333333332</v>
+        <v>9.2833333000000007</v>
       </c>
       <c r="C30" s="23">
         <v>0</v>
@@ -2782,9 +2782,9 @@
       <c r="L30" s="8"/>
     </row>
     <row r="31" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="102"/>
+      <c r="A31" s="101"/>
       <c r="B31" s="27">
-        <v>11.033333333333333</v>
+        <v>11.033333000000001</v>
       </c>
       <c r="C31" s="23">
         <v>1.0999999999999999E-2</v>
@@ -2810,7 +2810,7 @@
       <c r="L31" s="8"/>
     </row>
     <row r="32" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="102"/>
+      <c r="A32" s="101"/>
       <c r="B32" s="27">
         <v>13.15</v>
       </c>
@@ -2838,9 +2838,9 @@
       <c r="L32" s="8"/>
     </row>
     <row r="33" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="102"/>
+      <c r="A33" s="101"/>
       <c r="B33" s="27">
-        <v>15.150000000000002</v>
+        <v>15.15</v>
       </c>
       <c r="C33" s="23">
         <v>5.0000000000000001E-3</v>
@@ -2866,9 +2866,9 @@
       <c r="L33" s="8"/>
     </row>
     <row r="34" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="102"/>
+      <c r="A34" s="101"/>
       <c r="B34" s="27">
-        <v>17.100000000000005</v>
+        <v>17.100000000000001</v>
       </c>
       <c r="C34" s="23">
         <v>0</v>
@@ -2894,9 +2894,9 @@
       <c r="L34" s="8"/>
     </row>
     <row r="35" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="102"/>
+      <c r="A35" s="101"/>
       <c r="B35" s="27">
-        <v>18.150000000000002</v>
+        <v>18.149999999999999</v>
       </c>
       <c r="C35" s="23">
         <v>6.0000000000000001E-3</v>
@@ -2922,9 +2922,9 @@
       <c r="L35" s="8"/>
     </row>
     <row r="36" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="102"/>
+      <c r="A36" s="101"/>
       <c r="B36" s="27">
-        <v>19.166666666666668</v>
+        <v>19.166667</v>
       </c>
       <c r="C36" s="23">
         <v>8.9999999999999993E-3</v>
@@ -2950,9 +2950,9 @@
       <c r="L36" s="8"/>
     </row>
     <row r="37" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="102"/>
+      <c r="A37" s="101"/>
       <c r="B37" s="27">
-        <v>20.133333333333336</v>
+        <v>20.133333</v>
       </c>
       <c r="C37" s="23">
         <v>0</v>
@@ -2978,7 +2978,7 @@
       <c r="L37" s="75"/>
     </row>
     <row r="38" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="103" t="s">
+      <c r="A38" s="100" t="s">
         <v>105</v>
       </c>
       <c r="B38" s="29">
@@ -3008,9 +3008,9 @@
       <c r="L38" s="75"/>
     </row>
     <row r="39" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="103"/>
+      <c r="A39" s="100"/>
       <c r="B39" s="29">
-        <v>1.216666666666665</v>
+        <v>1.2166667</v>
       </c>
       <c r="C39" s="30">
         <v>7.9470000000000001</v>
@@ -3036,9 +3036,9 @@
       <c r="L39" s="75"/>
     </row>
     <row r="40" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="103"/>
+      <c r="A40" s="100"/>
       <c r="B40" s="29">
-        <v>2.0500000000000007</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="C40" s="30">
         <v>7.2729999999999997</v>
@@ -3064,9 +3064,9 @@
       <c r="L40" s="75"/>
     </row>
     <row r="41" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="103"/>
+      <c r="A41" s="100"/>
       <c r="B41" s="29">
-        <v>2.8333333333333304</v>
+        <v>2.8333333000000001</v>
       </c>
       <c r="C41" s="30">
         <v>5.6609999999999996</v>
@@ -3092,11 +3092,11 @@
       <c r="L41" s="75"/>
     </row>
     <row r="42" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="103" t="s">
+      <c r="A42" s="100" t="s">
         <v>104</v>
       </c>
       <c r="B42" s="29">
-        <v>5.2999999999999989</v>
+        <v>5.3</v>
       </c>
       <c r="C42" s="30">
         <v>0.29499999999999998</v>
@@ -3122,9 +3122,9 @@
       <c r="L42" s="75"/>
     </row>
     <row r="43" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="103"/>
+      <c r="A43" s="100"/>
       <c r="B43" s="29">
-        <v>6.9999999999999982</v>
+        <v>7</v>
       </c>
       <c r="C43" s="30">
         <v>0</v>
@@ -3150,9 +3150,9 @@
       <c r="L43" s="75"/>
     </row>
     <row r="44" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="103"/>
+      <c r="A44" s="100"/>
       <c r="B44" s="29">
-        <v>7.7333333333333361</v>
+        <v>7.7333333</v>
       </c>
       <c r="C44" s="30">
         <v>0</v>
@@ -3178,9 +3178,9 @@
       <c r="L44" s="75"/>
     </row>
     <row r="45" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="103"/>
+      <c r="A45" s="100"/>
       <c r="B45" s="29">
-        <v>8.6166666666666689</v>
+        <v>8.6166666999999997</v>
       </c>
       <c r="C45" s="30">
         <v>0</v>
@@ -3206,9 +3206,9 @@
       <c r="L45" s="75"/>
     </row>
     <row r="46" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="103"/>
+      <c r="A46" s="100"/>
       <c r="B46" s="29">
-        <v>9.2166666666666668</v>
+        <v>9.2166666999999993</v>
       </c>
       <c r="C46" s="30">
         <v>0</v>
@@ -3234,11 +3234,11 @@
       <c r="L46" s="75"/>
     </row>
     <row r="47" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="103" t="s">
+      <c r="A47" s="100" t="s">
         <v>103</v>
       </c>
       <c r="B47" s="34">
-        <v>10.499999999999998</v>
+        <v>10.5</v>
       </c>
       <c r="C47" s="30">
         <v>0</v>
@@ -3264,9 +3264,9 @@
       <c r="L47" s="7"/>
     </row>
     <row r="48" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="103"/>
+      <c r="A48" s="100"/>
       <c r="B48" s="36">
-        <v>12.249999999999998</v>
+        <v>12.25</v>
       </c>
       <c r="C48" s="30">
         <v>0</v>
@@ -3292,9 +3292,9 @@
       <c r="L48" s="8"/>
     </row>
     <row r="49" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="103"/>
+      <c r="A49" s="100"/>
       <c r="B49" s="36">
-        <v>14.366666666666665</v>
+        <v>14.366667</v>
       </c>
       <c r="C49" s="30">
         <v>0</v>
@@ -3320,9 +3320,9 @@
       <c r="L49" s="8"/>
     </row>
     <row r="50" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="103"/>
+      <c r="A50" s="100"/>
       <c r="B50" s="36">
-        <v>16.366666666666667</v>
+        <v>16.366667</v>
       </c>
       <c r="C50" s="30">
         <v>0</v>
@@ -3348,9 +3348,9 @@
       <c r="L50" s="8"/>
     </row>
     <row r="51" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="103"/>
+      <c r="A51" s="100"/>
       <c r="B51" s="36">
-        <v>18.299999999999997</v>
+        <v>18.3</v>
       </c>
       <c r="C51" s="30">
         <v>0</v>
@@ -3376,9 +3376,9 @@
       <c r="L51" s="8"/>
     </row>
     <row r="52" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="103"/>
+      <c r="A52" s="100"/>
       <c r="B52" s="36">
-        <v>19.366666666666667</v>
+        <v>19.366667</v>
       </c>
       <c r="C52" s="30">
         <v>0</v>
@@ -3404,7 +3404,7 @@
       <c r="L52" s="8"/>
     </row>
     <row r="53" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="104" t="s">
+      <c r="A53" s="103" t="s">
         <v>105</v>
       </c>
       <c r="B53" s="38">
@@ -3434,7 +3434,7 @@
       <c r="L53" s="8"/>
     </row>
     <row r="54" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="104"/>
+      <c r="A54" s="103"/>
       <c r="B54" s="38">
         <v>0.68333332999999996</v>
       </c>
@@ -3462,7 +3462,7 @@
       <c r="L54" s="74"/>
     </row>
     <row r="55" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="104"/>
+      <c r="A55" s="103"/>
       <c r="B55" s="38">
         <v>1.71666667</v>
       </c>
@@ -3490,7 +3490,7 @@
       <c r="L55" s="74"/>
     </row>
     <row r="56" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="104"/>
+      <c r="A56" s="103"/>
       <c r="B56" s="38">
         <v>2.15</v>
       </c>
@@ -3518,7 +3518,7 @@
       <c r="L56" s="74"/>
     </row>
     <row r="57" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="104"/>
+      <c r="A57" s="103"/>
       <c r="B57" s="38">
         <v>2.6666666700000001</v>
       </c>
@@ -3546,7 +3546,7 @@
       <c r="L57" s="74"/>
     </row>
     <row r="58" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="104"/>
+      <c r="A58" s="103"/>
       <c r="B58" s="38">
         <v>3.1666666700000001</v>
       </c>
@@ -3574,7 +3574,7 @@
       <c r="L58" s="74"/>
     </row>
     <row r="59" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="104"/>
+      <c r="A59" s="103"/>
       <c r="B59" s="38">
         <v>3.6666666700000001</v>
       </c>
@@ -3602,7 +3602,7 @@
       <c r="L59" s="74"/>
     </row>
     <row r="60" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="104"/>
+      <c r="A60" s="103"/>
       <c r="B60" s="38">
         <v>4.1666666699999997</v>
       </c>
@@ -3630,7 +3630,7 @@
       <c r="L60" s="74"/>
     </row>
     <row r="61" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="104" t="s">
+      <c r="A61" s="103" t="s">
         <v>104</v>
       </c>
       <c r="B61" s="38">
@@ -3660,7 +3660,7 @@
       <c r="L61" s="74"/>
     </row>
     <row r="62" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="104"/>
+      <c r="A62" s="103"/>
       <c r="B62" s="38">
         <v>5.55</v>
       </c>
@@ -3688,7 +3688,7 @@
       <c r="L62" s="74"/>
     </row>
     <row r="63" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="104"/>
+      <c r="A63" s="103"/>
       <c r="B63" s="38">
         <v>6.5</v>
       </c>
@@ -3716,7 +3716,7 @@
       <c r="L63" s="74"/>
     </row>
     <row r="64" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="104"/>
+      <c r="A64" s="103"/>
       <c r="B64" s="38">
         <v>7</v>
       </c>
@@ -3744,7 +3744,7 @@
       <c r="L64" s="74"/>
     </row>
     <row r="65" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="104"/>
+      <c r="A65" s="103"/>
       <c r="B65" s="38">
         <v>7.7166666700000004</v>
       </c>
@@ -3772,7 +3772,7 @@
       <c r="L65" s="74"/>
     </row>
     <row r="66" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="104"/>
+      <c r="A66" s="103"/>
       <c r="B66" s="38">
         <v>8.35</v>
       </c>
@@ -3800,7 +3800,7 @@
       <c r="L66" s="74"/>
     </row>
     <row r="67" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="104"/>
+      <c r="A67" s="103"/>
       <c r="B67" s="38">
         <v>8.9666666700000004</v>
       </c>
@@ -3828,7 +3828,7 @@
       <c r="L67" s="74"/>
     </row>
     <row r="68" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="104" t="s">
+      <c r="A68" s="103" t="s">
         <v>103</v>
       </c>
       <c r="B68" s="43">
@@ -3858,7 +3858,7 @@
       <c r="L68" s="74"/>
     </row>
     <row r="69" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="104"/>
+      <c r="A69" s="103"/>
       <c r="B69" s="43">
         <v>11.033333300000001</v>
       </c>
@@ -3886,7 +3886,7 @@
       <c r="L69" s="8"/>
     </row>
     <row r="70" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="104"/>
+      <c r="A70" s="103"/>
       <c r="B70" s="43">
         <v>11.966666699999999</v>
       </c>
@@ -3914,7 +3914,7 @@
       <c r="L70" s="8"/>
     </row>
     <row r="71" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="104"/>
+      <c r="A71" s="103"/>
       <c r="B71" s="43">
         <v>12.966666699999999</v>
       </c>
@@ -3942,7 +3942,7 @@
       <c r="L71" s="8"/>
     </row>
     <row r="72" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="104"/>
+      <c r="A72" s="103"/>
       <c r="B72" s="43">
         <v>14.05</v>
       </c>
@@ -3970,7 +3970,7 @@
       <c r="L72" s="8"/>
     </row>
     <row r="73" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="104"/>
+      <c r="A73" s="103"/>
       <c r="B73" s="43">
         <v>14.933333299999999</v>
       </c>
@@ -3998,7 +3998,7 @@
       <c r="L73" s="8"/>
     </row>
     <row r="74" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="101" t="s">
+      <c r="A74" s="99" t="s">
         <v>105</v>
       </c>
       <c r="B74" s="45">
@@ -4028,9 +4028,9 @@
       <c r="L74" s="8"/>
     </row>
     <row r="75" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="101"/>
+      <c r="A75" s="99"/>
       <c r="B75" s="45">
-        <v>0.68333333333333357</v>
+        <v>0.68333332999999996</v>
       </c>
       <c r="C75" s="46">
         <v>9.4599999999999991</v>
@@ -4056,9 +4056,9 @@
       <c r="L75" s="8"/>
     </row>
     <row r="76" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="101"/>
+      <c r="A76" s="99"/>
       <c r="B76" s="45">
-        <v>1.7166666666666659</v>
+        <v>1.71666667</v>
       </c>
       <c r="C76" s="46">
         <v>8.98</v>
@@ -4084,9 +4084,9 @@
       <c r="L76" s="8"/>
     </row>
     <row r="77" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="101"/>
+      <c r="A77" s="99"/>
       <c r="B77" s="45">
-        <v>2.1499999999999977</v>
+        <v>2.15</v>
       </c>
       <c r="C77" s="46">
         <v>8.17</v>
@@ -4112,9 +4112,9 @@
       <c r="L77" s="8"/>
     </row>
     <row r="78" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="101"/>
+      <c r="A78" s="99"/>
       <c r="B78" s="45">
-        <v>2.6166666666666654</v>
+        <v>2.6166666699999999</v>
       </c>
       <c r="C78" s="46">
         <v>7.71</v>
@@ -4140,9 +4140,9 @@
       <c r="L78" s="8"/>
     </row>
     <row r="79" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="101"/>
+      <c r="A79" s="99"/>
       <c r="B79" s="45">
-        <v>3.1666666666666661</v>
+        <v>3.1666666700000001</v>
       </c>
       <c r="C79" s="46">
         <v>7.24</v>
@@ -4168,9 +4168,9 @@
       <c r="L79" s="8"/>
     </row>
     <row r="80" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="101"/>
+      <c r="A80" s="99"/>
       <c r="B80" s="45">
-        <v>3.6666666666666652</v>
+        <v>3.6666666700000001</v>
       </c>
       <c r="C80" s="46">
         <v>5.08</v>
@@ -4196,9 +4196,9 @@
       <c r="L80" s="8"/>
     </row>
     <row r="81" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="101"/>
+      <c r="A81" s="99"/>
       <c r="B81" s="45">
-        <v>4.166666666666667</v>
+        <v>4.1666666699999997</v>
       </c>
       <c r="C81" s="46">
         <v>3.08</v>
@@ -4224,11 +4224,11 @@
       <c r="L81" s="8"/>
     </row>
     <row r="82" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="101" t="s">
+      <c r="A82" s="99" t="s">
         <v>104</v>
       </c>
       <c r="B82" s="45">
-        <v>5.8999999999999986</v>
+        <v>4.6500000000000004</v>
       </c>
       <c r="C82" s="46">
         <v>0.6</v>
@@ -4254,9 +4254,9 @@
       <c r="L82" s="8"/>
     </row>
     <row r="83" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="101"/>
+      <c r="A83" s="99"/>
       <c r="B83" s="45">
-        <v>6.7500000000000018</v>
+        <v>5.5</v>
       </c>
       <c r="C83" s="46">
         <v>1.2E-2</v>
@@ -4282,9 +4282,9 @@
       <c r="L83" s="8"/>
     </row>
     <row r="84" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="101"/>
+      <c r="A84" s="99"/>
       <c r="B84" s="45">
-        <v>7.75</v>
+        <v>6.5</v>
       </c>
       <c r="C84" s="46">
         <v>0.159</v>
@@ -4310,9 +4310,9 @@
       <c r="L84" s="8"/>
     </row>
     <row r="85" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="101"/>
+      <c r="A85" s="99"/>
       <c r="B85" s="45">
-        <v>8.2500000000000018</v>
+        <v>7</v>
       </c>
       <c r="C85" s="46">
         <v>1.2E-2</v>
@@ -4338,9 +4338,9 @@
       <c r="L85" s="8"/>
     </row>
     <row r="86" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="101"/>
+      <c r="A86" s="99"/>
       <c r="B86" s="45">
-        <v>8.9666666666666686</v>
+        <v>7.7166666700000004</v>
       </c>
       <c r="C86" s="46">
         <v>1.0999999999999999E-2</v>
@@ -4366,9 +4366,9 @@
       <c r="L86" s="8"/>
     </row>
     <row r="87" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="101"/>
+      <c r="A87" s="99"/>
       <c r="B87" s="45">
-        <v>9.6</v>
+        <v>8.35</v>
       </c>
       <c r="C87" s="46">
         <v>8.0000000000000002E-3</v>
@@ -4394,9 +4394,9 @@
       <c r="L87" s="8"/>
     </row>
     <row r="88" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="101"/>
+      <c r="A88" s="99"/>
       <c r="B88" s="45">
-        <v>10.316666666666666</v>
+        <v>9.06666667</v>
       </c>
       <c r="C88" s="46">
         <v>1.4999999999999999E-2</v>
@@ -4422,11 +4422,11 @@
       <c r="L88" s="8"/>
     </row>
     <row r="89" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="101" t="s">
+      <c r="A89" s="99" t="s">
         <v>103</v>
       </c>
       <c r="B89" s="45">
-        <v>9.9333333333333318</v>
+        <v>9.93333333</v>
       </c>
       <c r="C89" s="46">
         <v>1.0999999999999999E-2</v>
@@ -4452,9 +4452,9 @@
       <c r="L89" s="8"/>
     </row>
     <row r="90" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="101"/>
+      <c r="A90" s="99"/>
       <c r="B90" s="45">
-        <v>11.033333333333333</v>
+        <v>11.033333300000001</v>
       </c>
       <c r="C90" s="46">
         <v>0</v>
@@ -4480,9 +4480,9 @@
       <c r="L90" s="8"/>
     </row>
     <row r="91" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="101"/>
+      <c r="A91" s="99"/>
       <c r="B91" s="45">
-        <v>11.999999999999998</v>
+        <v>12</v>
       </c>
       <c r="C91" s="46">
         <v>8.9999999999999993E-3</v>
@@ -4508,9 +4508,9 @@
       <c r="L91" s="8"/>
     </row>
     <row r="92" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="101"/>
+      <c r="A92" s="99"/>
       <c r="B92" s="45">
-        <v>12.999999999999998</v>
+        <v>13</v>
       </c>
       <c r="C92" s="46">
         <v>0.01</v>
@@ -4536,9 +4536,9 @@
       <c r="L92" s="8"/>
     </row>
     <row r="93" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="101"/>
+      <c r="A93" s="99"/>
       <c r="B93" s="45">
-        <v>14.049999999999999</v>
+        <v>14.05</v>
       </c>
       <c r="C93" s="46">
         <v>0</v>
@@ -4564,9 +4564,9 @@
       <c r="L93" s="8"/>
     </row>
     <row r="94" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="101"/>
+      <c r="A94" s="99"/>
       <c r="B94" s="45">
-        <v>14.916666666666666</v>
+        <v>14.9166667</v>
       </c>
       <c r="C94" s="46">
         <v>1.0999999999999999E-2</v>
@@ -4592,7 +4592,7 @@
       <c r="L94" s="8"/>
     </row>
     <row r="95" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="100" t="s">
+      <c r="A95" s="102" t="s">
         <v>105</v>
       </c>
       <c r="B95" s="48">
@@ -4622,7 +4622,7 @@
       <c r="L95" s="8"/>
     </row>
     <row r="96" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="100"/>
+      <c r="A96" s="102"/>
       <c r="B96" s="48">
         <v>0.75</v>
       </c>
@@ -4650,7 +4650,7 @@
       <c r="L96" s="8"/>
     </row>
     <row r="97" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="100"/>
+      <c r="A97" s="102"/>
       <c r="B97" s="48">
         <v>1.4166666699999999</v>
       </c>
@@ -4678,7 +4678,7 @@
       <c r="L97" s="8"/>
     </row>
     <row r="98" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="100"/>
+      <c r="A98" s="102"/>
       <c r="B98" s="48">
         <v>2.0833333299999999</v>
       </c>
@@ -4706,7 +4706,7 @@
       <c r="L98" s="8"/>
     </row>
     <row r="99" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="100"/>
+      <c r="A99" s="102"/>
       <c r="B99" s="48">
         <v>2.75</v>
       </c>
@@ -4734,7 +4734,7 @@
       <c r="L99" s="8"/>
     </row>
     <row r="100" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="100"/>
+      <c r="A100" s="102"/>
       <c r="B100" s="48">
         <v>3.5833333299999999</v>
       </c>
@@ -4762,7 +4762,7 @@
       <c r="L100" s="8"/>
     </row>
     <row r="101" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="100"/>
+      <c r="A101" s="102"/>
       <c r="B101" s="48">
         <v>4.5333333299999996</v>
       </c>
@@ -4790,7 +4790,7 @@
       <c r="L101" s="8"/>
     </row>
     <row r="102" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="100" t="s">
+      <c r="A102" s="102" t="s">
         <v>104</v>
       </c>
       <c r="B102" s="48">
@@ -4820,7 +4820,7 @@
       <c r="L102" s="8"/>
     </row>
     <row r="103" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="100"/>
+      <c r="A103" s="102"/>
       <c r="B103" s="48">
         <v>6.25</v>
       </c>
@@ -4848,7 +4848,7 @@
       <c r="L103" s="8"/>
     </row>
     <row r="104" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="100"/>
+      <c r="A104" s="102"/>
       <c r="B104" s="48">
         <v>7.5</v>
       </c>
@@ -4876,7 +4876,7 @@
       <c r="L104" s="8"/>
     </row>
     <row r="105" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="100"/>
+      <c r="A105" s="102"/>
       <c r="B105" s="48">
         <v>8.3333333300000003</v>
       </c>
@@ -4904,7 +4904,7 @@
       <c r="L105" s="8"/>
     </row>
     <row r="106" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="100"/>
+      <c r="A106" s="102"/>
       <c r="B106" s="48">
         <v>8.7833333299999996</v>
       </c>
@@ -4932,7 +4932,7 @@
       <c r="L106" s="8"/>
     </row>
     <row r="107" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="100" t="s">
+      <c r="A107" s="102" t="s">
         <v>103</v>
       </c>
       <c r="B107" s="48">
@@ -4962,7 +4962,7 @@
       <c r="L107" s="8"/>
     </row>
     <row r="108" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="100"/>
+      <c r="A108" s="102"/>
       <c r="B108" s="48">
         <v>11.1166667</v>
       </c>
@@ -4990,7 +4990,7 @@
       <c r="L108" s="8"/>
     </row>
     <row r="109" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="100"/>
+      <c r="A109" s="102"/>
       <c r="B109" s="48">
         <v>12</v>
       </c>
@@ -5018,7 +5018,7 @@
       <c r="L109" s="8"/>
     </row>
     <row r="110" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="100"/>
+      <c r="A110" s="102"/>
       <c r="B110" s="48">
         <v>12.9166667</v>
       </c>
@@ -5046,7 +5046,7 @@
       <c r="L110" s="8"/>
     </row>
     <row r="111" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="100"/>
+      <c r="A111" s="102"/>
       <c r="B111" s="48">
         <v>14.1666667</v>
       </c>
@@ -5074,7 +5074,7 @@
       <c r="L111" s="8"/>
     </row>
     <row r="112" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="100"/>
+      <c r="A112" s="102"/>
       <c r="B112" s="48">
         <v>15.75</v>
       </c>
@@ -5102,7 +5102,7 @@
       <c r="L112" s="8"/>
     </row>
     <row r="113" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="100"/>
+      <c r="A113" s="102"/>
       <c r="B113" s="48">
         <v>17.75</v>
       </c>
@@ -5130,7 +5130,7 @@
       <c r="L113" s="8"/>
     </row>
     <row r="114" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="100"/>
+      <c r="A114" s="102"/>
       <c r="B114" s="48">
         <v>22.0833333</v>
       </c>
@@ -5158,7 +5158,7 @@
       <c r="L114" s="8"/>
     </row>
     <row r="115" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="100"/>
+      <c r="A115" s="102"/>
       <c r="B115" s="48">
         <v>23.75</v>
       </c>
@@ -5186,7 +5186,7 @@
       <c r="L115" s="8"/>
     </row>
     <row r="116" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="100"/>
+      <c r="A116" s="102"/>
       <c r="B116" s="48">
         <v>26.25</v>
       </c>
@@ -5214,7 +5214,7 @@
       <c r="L116" s="8"/>
     </row>
     <row r="117" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="100"/>
+      <c r="A117" s="102"/>
       <c r="B117" s="48">
         <v>27.9166667</v>
       </c>
@@ -5242,7 +5242,7 @@
       <c r="L117" s="8"/>
     </row>
     <row r="118" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="100"/>
+      <c r="A118" s="102"/>
       <c r="B118" s="48">
         <v>30.783333299999999</v>
       </c>
@@ -5270,7 +5270,7 @@
       <c r="L118" s="8"/>
     </row>
     <row r="119" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="100"/>
+      <c r="A119" s="102"/>
       <c r="B119" s="48">
         <v>33.716666699999998</v>
       </c>
@@ -5298,7 +5298,7 @@
       <c r="L119" s="8"/>
     </row>
     <row r="120" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="100"/>
+      <c r="A120" s="102"/>
       <c r="B120" s="48">
         <v>36.75</v>
       </c>
@@ -5326,7 +5326,7 @@
       <c r="L120" s="8"/>
     </row>
     <row r="121" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="100"/>
+      <c r="A121" s="102"/>
       <c r="B121" s="48">
         <v>39.25</v>
       </c>
@@ -5354,7 +5354,7 @@
       <c r="L121" s="8"/>
     </row>
     <row r="122" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="100"/>
+      <c r="A122" s="102"/>
       <c r="B122" s="48">
         <v>46.533333300000002</v>
       </c>
@@ -5382,7 +5382,7 @@
       <c r="L122" s="8"/>
     </row>
     <row r="123" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="102" t="s">
+      <c r="A123" s="101" t="s">
         <v>105</v>
       </c>
       <c r="B123" s="27">
@@ -5412,7 +5412,7 @@
       <c r="L123" s="8"/>
     </row>
     <row r="124" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="102"/>
+      <c r="A124" s="101"/>
       <c r="B124" s="27">
         <v>0.65</v>
       </c>
@@ -5440,7 +5440,7 @@
       <c r="L124" s="8"/>
     </row>
     <row r="125" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="102"/>
+      <c r="A125" s="101"/>
       <c r="B125" s="27">
         <v>1.3833333299999999</v>
       </c>
@@ -5468,7 +5468,7 @@
       <c r="L125" s="8"/>
     </row>
     <row r="126" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="102"/>
+      <c r="A126" s="101"/>
       <c r="B126" s="27">
         <v>2.15</v>
       </c>
@@ -5496,7 +5496,7 @@
       <c r="L126" s="8"/>
     </row>
     <row r="127" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="102"/>
+      <c r="A127" s="101"/>
       <c r="B127" s="27">
         <v>2.7333333299999998</v>
       </c>
@@ -5524,7 +5524,7 @@
       <c r="L127" s="8"/>
     </row>
     <row r="128" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="102"/>
+      <c r="A128" s="101"/>
       <c r="B128" s="27">
         <v>3.6333333300000001</v>
       </c>
@@ -5552,7 +5552,7 @@
       <c r="L128" s="8"/>
     </row>
     <row r="129" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="102" t="s">
+      <c r="A129" s="101" t="s">
         <v>104</v>
       </c>
       <c r="B129" s="27">
@@ -5582,7 +5582,7 @@
       <c r="L129" s="8"/>
     </row>
     <row r="130" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="102"/>
+      <c r="A130" s="101"/>
       <c r="B130" s="27">
         <v>5.55</v>
       </c>
@@ -5610,7 +5610,7 @@
       <c r="L130" s="8"/>
     </row>
     <row r="131" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="102"/>
+      <c r="A131" s="101"/>
       <c r="B131" s="27">
         <v>6.18333333</v>
       </c>
@@ -5638,7 +5638,7 @@
       <c r="L131" s="8"/>
     </row>
     <row r="132" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="102"/>
+      <c r="A132" s="101"/>
       <c r="B132" s="27">
         <v>7.45</v>
       </c>
@@ -5666,7 +5666,7 @@
       <c r="L132" s="8"/>
     </row>
     <row r="133" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="102"/>
+      <c r="A133" s="101"/>
       <c r="B133" s="27">
         <v>8.35</v>
       </c>
@@ -5694,7 +5694,7 @@
       <c r="L133" s="8"/>
     </row>
     <row r="134" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="102"/>
+      <c r="A134" s="101"/>
       <c r="B134" s="27">
         <v>9.35</v>
       </c>
@@ -5722,7 +5722,7 @@
       <c r="L134" s="8"/>
     </row>
     <row r="135" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="102"/>
+      <c r="A135" s="101"/>
       <c r="B135" s="27">
         <v>10.5</v>
       </c>
@@ -5750,7 +5750,7 @@
       <c r="L135" s="8"/>
     </row>
     <row r="136" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="102"/>
+      <c r="A136" s="101"/>
       <c r="B136" s="27">
         <v>11.9166667</v>
       </c>
@@ -5778,7 +5778,7 @@
       <c r="L136" s="8"/>
     </row>
     <row r="137" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="102" t="s">
+      <c r="A137" s="101" t="s">
         <v>103</v>
       </c>
       <c r="B137" s="27">
@@ -5808,7 +5808,7 @@
       <c r="L137" s="8"/>
     </row>
     <row r="138" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="102"/>
+      <c r="A138" s="101"/>
       <c r="B138" s="27">
         <v>14.25</v>
       </c>
@@ -5836,7 +5836,7 @@
       <c r="L138" s="8"/>
     </row>
     <row r="139" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="102"/>
+      <c r="A139" s="101"/>
       <c r="B139" s="27">
         <v>15.75</v>
       </c>
@@ -5864,7 +5864,7 @@
       <c r="L139" s="8"/>
     </row>
     <row r="140" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="102"/>
+      <c r="A140" s="101"/>
       <c r="B140" s="27">
         <v>17.75</v>
       </c>
@@ -5892,7 +5892,7 @@
       <c r="L140" s="8"/>
     </row>
     <row r="141" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="102"/>
+      <c r="A141" s="101"/>
       <c r="B141" s="27">
         <v>22.0833333</v>
       </c>
@@ -5920,7 +5920,7 @@
       <c r="L141" s="8"/>
     </row>
     <row r="142" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="102"/>
+      <c r="A142" s="101"/>
       <c r="B142" s="27">
         <v>23.75</v>
       </c>
@@ -5948,7 +5948,7 @@
       <c r="L142" s="8"/>
     </row>
     <row r="143" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="102"/>
+      <c r="A143" s="101"/>
       <c r="B143" s="27">
         <v>26.25</v>
       </c>
@@ -5976,7 +5976,7 @@
       <c r="L143" s="8"/>
     </row>
     <row r="144" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="102"/>
+      <c r="A144" s="101"/>
       <c r="B144" s="27">
         <v>27.9166667</v>
       </c>
@@ -6004,7 +6004,7 @@
       <c r="L144" s="8"/>
     </row>
     <row r="145" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="102"/>
+      <c r="A145" s="101"/>
       <c r="B145" s="27">
         <v>30.7</v>
       </c>
@@ -6032,7 +6032,7 @@
       <c r="L145" s="8"/>
     </row>
     <row r="146" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="102"/>
+      <c r="A146" s="101"/>
       <c r="B146" s="27">
         <v>33.75</v>
       </c>
@@ -6060,7 +6060,7 @@
       <c r="L146" s="8"/>
     </row>
     <row r="147" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="102"/>
+      <c r="A147" s="101"/>
       <c r="B147" s="27">
         <v>36.75</v>
       </c>
@@ -6088,7 +6088,7 @@
       <c r="L147" s="8"/>
     </row>
     <row r="148" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="102"/>
+      <c r="A148" s="101"/>
       <c r="B148" s="27">
         <v>39.3333333</v>
       </c>
@@ -6116,7 +6116,7 @@
       <c r="L148" s="8"/>
     </row>
     <row r="149" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="102"/>
+      <c r="A149" s="101"/>
       <c r="B149" s="27">
         <v>46.933333300000001</v>
       </c>
@@ -6144,7 +6144,7 @@
       <c r="L149" s="8"/>
     </row>
     <row r="150" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="101" t="s">
+      <c r="A150" s="99" t="s">
         <v>105</v>
       </c>
       <c r="B150" s="45">
@@ -6174,7 +6174,7 @@
       <c r="L150" s="8"/>
     </row>
     <row r="151" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="101"/>
+      <c r="A151" s="99"/>
       <c r="B151" s="45">
         <v>0.8</v>
       </c>
@@ -6202,7 +6202,7 @@
       <c r="L151" s="8"/>
     </row>
     <row r="152" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="101"/>
+      <c r="A152" s="99"/>
       <c r="B152" s="45">
         <v>1.85</v>
       </c>
@@ -6230,7 +6230,7 @@
       <c r="L152" s="8"/>
     </row>
     <row r="153" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="101"/>
+      <c r="A153" s="99"/>
       <c r="B153" s="45">
         <v>3.03333333</v>
       </c>
@@ -6258,7 +6258,7 @@
       <c r="L153" s="8"/>
     </row>
     <row r="154" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="101" t="s">
+      <c r="A154" s="99" t="s">
         <v>104</v>
       </c>
       <c r="B154" s="45">
@@ -6288,7 +6288,7 @@
       <c r="L154" s="8"/>
     </row>
     <row r="155" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="101"/>
+      <c r="A155" s="99"/>
       <c r="B155" s="45">
         <v>4.9666666700000004</v>
       </c>
@@ -6316,7 +6316,7 @@
       <c r="L155" s="8"/>
     </row>
     <row r="156" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="101"/>
+      <c r="A156" s="99"/>
       <c r="B156" s="45">
         <v>5.8333333300000003</v>
       </c>
@@ -6344,7 +6344,7 @@
       <c r="L156" s="8"/>
     </row>
     <row r="157" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="101"/>
+      <c r="A157" s="99"/>
       <c r="B157" s="45">
         <v>6.9166666699999997</v>
       </c>
@@ -6372,7 +6372,7 @@
       <c r="L157" s="8"/>
     </row>
     <row r="158" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="101"/>
+      <c r="A158" s="99"/>
       <c r="B158" s="45">
         <v>7.6333333300000001</v>
       </c>
@@ -6400,7 +6400,7 @@
       <c r="L158" s="8"/>
     </row>
     <row r="159" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="101"/>
+      <c r="A159" s="99"/>
       <c r="B159" s="45">
         <v>8.25</v>
       </c>
@@ -6428,7 +6428,7 @@
       <c r="L159" s="8"/>
     </row>
     <row r="160" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="101"/>
+      <c r="A160" s="99"/>
       <c r="B160" s="45">
         <v>9.0500000000000007</v>
       </c>
@@ -6456,7 +6456,7 @@
       <c r="L160" s="8"/>
     </row>
     <row r="161" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="101" t="s">
+      <c r="A161" s="99" t="s">
         <v>103</v>
       </c>
       <c r="B161" s="45">
@@ -6486,7 +6486,7 @@
       <c r="L161" s="8"/>
     </row>
     <row r="162" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="101"/>
+      <c r="A162" s="99"/>
       <c r="B162" s="45">
         <v>11.566666700000001</v>
       </c>
@@ -6514,7 +6514,7 @@
       <c r="L162" s="8"/>
     </row>
     <row r="163" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="101"/>
+      <c r="A163" s="99"/>
       <c r="B163" s="45">
         <v>12.6666667</v>
       </c>
@@ -6542,7 +6542,7 @@
       <c r="L163" s="8"/>
     </row>
     <row r="164" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A164" s="101"/>
+      <c r="A164" s="99"/>
       <c r="B164" s="45">
         <v>14.1333333</v>
       </c>
@@ -6570,7 +6570,7 @@
       <c r="L164" s="8"/>
     </row>
     <row r="165" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="101"/>
+      <c r="A165" s="99"/>
       <c r="B165" s="45">
         <v>16.850000000000001</v>
       </c>
@@ -6598,7 +6598,7 @@
       <c r="L165" s="8"/>
     </row>
     <row r="166" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="101"/>
+      <c r="A166" s="99"/>
       <c r="B166" s="45">
         <v>22.4</v>
       </c>
@@ -6626,7 +6626,7 @@
       <c r="L166" s="8"/>
     </row>
     <row r="167" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A167" s="101"/>
+      <c r="A167" s="99"/>
       <c r="B167" s="45">
         <v>24.05</v>
       </c>
@@ -6654,7 +6654,7 @@
       <c r="L167" s="8"/>
     </row>
     <row r="168" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A168" s="101"/>
+      <c r="A168" s="99"/>
       <c r="B168" s="45">
         <v>25.55</v>
       </c>
@@ -6682,7 +6682,7 @@
       <c r="L168" s="8"/>
     </row>
     <row r="169" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A169" s="101"/>
+      <c r="A169" s="99"/>
       <c r="B169" s="45">
         <v>27.016666699999998</v>
       </c>
@@ -6710,7 +6710,7 @@
       <c r="L169" s="8"/>
     </row>
     <row r="170" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A170" s="101"/>
+      <c r="A170" s="99"/>
       <c r="B170" s="45">
         <v>30.05</v>
       </c>
@@ -6738,7 +6738,7 @@
       <c r="L170" s="8"/>
     </row>
     <row r="171" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A171" s="101"/>
+      <c r="A171" s="99"/>
       <c r="B171" s="45">
         <v>33.049999999999997</v>
       </c>
@@ -6766,7 +6766,7 @@
       <c r="L171" s="8"/>
     </row>
     <row r="172" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A172" s="101"/>
+      <c r="A172" s="99"/>
       <c r="B172" s="45">
         <v>35.716666699999998</v>
       </c>
@@ -6794,7 +6794,7 @@
       <c r="L172" s="8"/>
     </row>
     <row r="173" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A173" s="101"/>
+      <c r="A173" s="99"/>
       <c r="B173" s="45">
         <v>38.4166667</v>
       </c>
@@ -6822,7 +6822,7 @@
       <c r="L173" s="8"/>
     </row>
     <row r="174" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A174" s="101"/>
+      <c r="A174" s="99"/>
       <c r="B174" s="45">
         <v>46.4166667</v>
       </c>
@@ -6850,7 +6850,7 @@
       <c r="L174" s="8"/>
     </row>
     <row r="175" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A175" s="99" t="s">
+      <c r="A175" s="104" t="s">
         <v>105</v>
       </c>
       <c r="B175" s="17">
@@ -6880,7 +6880,7 @@
       <c r="L175" s="8"/>
     </row>
     <row r="176" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A176" s="99"/>
+      <c r="A176" s="104"/>
       <c r="B176" s="17">
         <v>1.1333333299999999</v>
       </c>
@@ -6908,7 +6908,7 @@
       <c r="L176" s="8"/>
     </row>
     <row r="177" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A177" s="99"/>
+      <c r="A177" s="104"/>
       <c r="B177" s="17">
         <v>1.95</v>
       </c>
@@ -6936,7 +6936,7 @@
       <c r="L177" s="8"/>
     </row>
     <row r="178" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A178" s="99"/>
+      <c r="A178" s="104"/>
       <c r="B178" s="17">
         <v>2.95</v>
       </c>
@@ -6964,7 +6964,7 @@
       <c r="L178" s="8"/>
     </row>
     <row r="179" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A179" s="99" t="s">
+      <c r="A179" s="104" t="s">
         <v>104</v>
       </c>
       <c r="B179" s="19">
@@ -6994,7 +6994,7 @@
       <c r="L179" s="8"/>
     </row>
     <row r="180" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A180" s="99"/>
+      <c r="A180" s="104"/>
       <c r="B180" s="19">
         <v>5.1333333300000001</v>
       </c>
@@ -7022,7 +7022,7 @@
       <c r="L180" s="8"/>
     </row>
     <row r="181" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A181" s="99"/>
+      <c r="A181" s="104"/>
       <c r="B181" s="19">
         <v>6.1333333300000001</v>
       </c>
@@ -7050,7 +7050,7 @@
       <c r="L181" s="8"/>
     </row>
     <row r="182" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A182" s="99"/>
+      <c r="A182" s="104"/>
       <c r="B182" s="19">
         <v>7</v>
       </c>
@@ -7078,7 +7078,7 @@
       <c r="L182" s="8"/>
     </row>
     <row r="183" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A183" s="99"/>
+      <c r="A183" s="104"/>
       <c r="B183" s="19">
         <v>8.0333333299999996</v>
       </c>
@@ -7106,7 +7106,7 @@
       <c r="L183" s="8"/>
     </row>
     <row r="184" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A184" s="99"/>
+      <c r="A184" s="104"/>
       <c r="B184" s="19">
         <v>8.65</v>
       </c>
@@ -7134,7 +7134,7 @@
       <c r="L184" s="8"/>
     </row>
     <row r="185" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A185" s="99"/>
+      <c r="A185" s="104"/>
       <c r="B185" s="19">
         <v>9.35</v>
       </c>
@@ -7162,7 +7162,7 @@
       <c r="L185" s="8"/>
     </row>
     <row r="186" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A186" s="99" t="s">
+      <c r="A186" s="104" t="s">
         <v>103</v>
       </c>
       <c r="B186" s="17">
@@ -7192,7 +7192,7 @@
       <c r="L186" s="8"/>
     </row>
     <row r="187" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A187" s="99"/>
+      <c r="A187" s="104"/>
       <c r="B187" s="17">
         <v>11.2</v>
       </c>
@@ -7220,7 +7220,7 @@
       <c r="L187" s="73"/>
     </row>
     <row r="188" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A188" s="99"/>
+      <c r="A188" s="104"/>
       <c r="B188" s="17">
         <v>12.6666667</v>
       </c>
@@ -7248,7 +7248,7 @@
       <c r="L188" s="73"/>
     </row>
     <row r="189" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A189" s="99"/>
+      <c r="A189" s="104"/>
       <c r="B189" s="17">
         <v>13.85</v>
       </c>
@@ -7276,7 +7276,7 @@
       <c r="L189" s="73"/>
     </row>
     <row r="190" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A190" s="99"/>
+      <c r="A190" s="104"/>
       <c r="B190" s="17">
         <v>15.316666700000001</v>
       </c>
@@ -7304,7 +7304,7 @@
       <c r="L190" s="73"/>
     </row>
     <row r="191" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A191" s="99"/>
+      <c r="A191" s="104"/>
       <c r="B191" s="17">
         <v>17.983333300000002</v>
       </c>
@@ -7332,7 +7332,7 @@
       <c r="L191" s="73"/>
     </row>
     <row r="192" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A192" s="99"/>
+      <c r="A192" s="104"/>
       <c r="B192" s="17">
         <v>23.566666699999999</v>
       </c>
@@ -7360,7 +7360,7 @@
       <c r="L192" s="73"/>
     </row>
     <row r="193" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A193" s="99"/>
+      <c r="A193" s="104"/>
       <c r="B193" s="17">
         <v>25.1333333</v>
       </c>
@@ -7388,7 +7388,7 @@
       <c r="L193" s="8"/>
     </row>
     <row r="194" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A194" s="99"/>
+      <c r="A194" s="104"/>
       <c r="B194" s="17">
         <v>26.683333300000001</v>
       </c>
@@ -7416,7 +7416,7 @@
       <c r="L194" s="8"/>
     </row>
     <row r="195" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A195" s="99"/>
+      <c r="A195" s="104"/>
       <c r="B195" s="17">
         <v>28.15</v>
       </c>
@@ -7444,7 +7444,7 @@
       <c r="L195" s="8"/>
     </row>
     <row r="196" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A196" s="99"/>
+      <c r="A196" s="104"/>
       <c r="B196" s="17">
         <v>31.183333300000001</v>
       </c>
@@ -7472,7 +7472,7 @@
       <c r="L196" s="8"/>
     </row>
     <row r="197" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A197" s="99"/>
+      <c r="A197" s="104"/>
       <c r="B197" s="17">
         <v>34.183333300000001</v>
       </c>
@@ -7500,7 +7500,7 @@
       <c r="L197" s="8"/>
     </row>
     <row r="198" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A198" s="99"/>
+      <c r="A198" s="104"/>
       <c r="B198" s="17">
         <v>35.700000000000003</v>
       </c>
@@ -7528,7 +7528,7 @@
       <c r="L198" s="8"/>
     </row>
     <row r="199" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A199" s="99"/>
+      <c r="A199" s="104"/>
       <c r="B199" s="17">
         <v>36.75</v>
       </c>
@@ -7581,21 +7581,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A2:A9"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="A10:A20"/>
-    <mergeCell ref="A30:A37"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="A42:A46"/>
-    <mergeCell ref="A47:A52"/>
-    <mergeCell ref="A82:A88"/>
-    <mergeCell ref="A89:A94"/>
-    <mergeCell ref="A95:A101"/>
-    <mergeCell ref="A53:A60"/>
-    <mergeCell ref="A61:A67"/>
-    <mergeCell ref="A68:A73"/>
-    <mergeCell ref="A74:A81"/>
     <mergeCell ref="A186:A199"/>
     <mergeCell ref="A102:A106"/>
     <mergeCell ref="A175:A178"/>
@@ -7607,6 +7592,21 @@
     <mergeCell ref="A129:A136"/>
     <mergeCell ref="A137:A149"/>
     <mergeCell ref="A107:A122"/>
+    <mergeCell ref="A42:A46"/>
+    <mergeCell ref="A47:A52"/>
+    <mergeCell ref="A82:A88"/>
+    <mergeCell ref="A89:A94"/>
+    <mergeCell ref="A95:A101"/>
+    <mergeCell ref="A53:A60"/>
+    <mergeCell ref="A61:A67"/>
+    <mergeCell ref="A68:A73"/>
+    <mergeCell ref="A74:A81"/>
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="A10:A20"/>
+    <mergeCell ref="A30:A37"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="A25:A29"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7618,8 +7618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFA57A6F-77E9-4760-888B-9ADD24B47B39}">
   <dimension ref="A1:F97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K79" sqref="K79"/>
+    <sheetView topLeftCell="A61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8405,7 +8405,7 @@
         <v>42</v>
       </c>
       <c r="B38" s="76">
-        <v>5.9</v>
+        <v>4.6500000000000004</v>
       </c>
       <c r="C38" s="92">
         <v>2.0258190963177389</v>
@@ -8426,7 +8426,7 @@
       </c>
       <c r="B39" s="94">
         <f>B38+C38</f>
-        <v>7.9258190963177393</v>
+        <v>6.6758190963177393</v>
       </c>
       <c r="C39" s="92">
         <v>0.62492948794595193</v>
@@ -8447,7 +8447,7 @@
       </c>
       <c r="B40" s="94">
         <f t="shared" ref="B40:B46" si="4">B39+C39</f>
-        <v>8.5507485842636903</v>
+        <v>7.3007485842636912</v>
       </c>
       <c r="C40" s="92">
         <v>0.38165100848674172</v>
@@ -8468,7 +8468,7 @@
       </c>
       <c r="B41" s="94">
         <f t="shared" si="4"/>
-        <v>8.932399592750432</v>
+        <v>7.6823995927504329</v>
       </c>
       <c r="C41" s="92">
         <v>0.27555892332417287</v>
@@ -8489,7 +8489,7 @@
       </c>
       <c r="B42" s="94">
         <f t="shared" si="4"/>
-        <v>9.2079585160746049</v>
+        <v>7.9579585160746058</v>
       </c>
       <c r="C42" s="92">
         <v>0.21579848280571667</v>
@@ -8510,7 +8510,7 @@
       </c>
       <c r="B43" s="94">
         <f t="shared" si="4"/>
-        <v>9.4237569988803216</v>
+        <v>8.1737569988803216</v>
       </c>
       <c r="C43" s="92">
         <v>0.17739469994920398</v>
@@ -8531,7 +8531,7 @@
       </c>
       <c r="B44" s="94">
         <f t="shared" si="4"/>
-        <v>9.6011516988295256</v>
+        <v>8.3511516988295256</v>
       </c>
       <c r="C44" s="92">
         <v>0.15061657525793137</v>
@@ -8552,7 +8552,7 @@
       </c>
       <c r="B45" s="94">
         <f t="shared" si="4"/>
-        <v>9.7517682740874569</v>
+        <v>8.5017682740874569</v>
       </c>
       <c r="C45" s="92">
         <v>0.13087259348850644</v>
@@ -8573,7 +8573,7 @@
       </c>
       <c r="B46" s="94">
         <f t="shared" si="4"/>
-        <v>9.8826408675759634</v>
+        <v>8.6326408675759634</v>
       </c>
       <c r="C46" s="92">
         <v>0.55159999999999998</v>
@@ -8594,7 +8594,7 @@
       </c>
       <c r="B47" s="94">
         <f>B46+C46</f>
-        <v>10.434240867575964</v>
+        <v>9.1842408675759639</v>
       </c>
       <c r="C47" s="92">
         <v>6.04</v>

</xml_diff>